<commit_message>
Level 0A doc and tdn data
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220627_Readme_NPOC_TN_COMPASS_TEMPEST_PW_n17.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220627_Readme_NPOC_TN_COMPASS_TEMPEST_PW_n17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/OneDrive - PNNL/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1673D6B-CAD6-DD4C-A8BC-9A015F3603A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E2287-E5E0-2645-9AFA-508F9EAC2447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31460" yWindow="4520" windowWidth="27660" windowHeight="15580" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Sample Name</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>CKSTD7_10ppm_C</t>
+  </si>
+  <si>
+    <t>Dilution correction needed</t>
   </si>
 </sst>
 </file>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AEBD17-6CC0-ED44-B8EB-00F06462890B}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,6 +848,9 @@
       </c>
       <c r="B27">
         <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -1315,15 +1321,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007324DF9BA5F6B948938C142504C8F34F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4aadcd1f2a12dc9b07f6546b5e76248">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da8c28ad-5ac5-4047-b08a-f75bc24d91a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6457694f174ba676422feeebbff24cf4" ns2:_="">
     <xsd:import namespace="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
@@ -1493,15 +1490,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A701949D-1257-47EA-88EF-D14148793769}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1517,4 +1515,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create Agu 2022 exploratory figures.Rmd and Update Readmes
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220627_Readme_NPOC_TN_COMPASS_TEMPEST_PW_n17.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220627_Readme_NPOC_TN_COMPASS_TEMPEST_PW_n17.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25524"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/OneDrive - PNNL/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oten406/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E2287-E5E0-2645-9AFA-508F9EAC2447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D0EFED8F-2FA7-0644-8684-9550ED20F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46117FC8-55FE-4AD4-A7A5-58C7345BE169}"/>
   <bookViews>
     <workbookView xWindow="31460" yWindow="4520" windowWidth="27660" windowHeight="15580" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Dilution sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Sample Name</t>
   </si>
@@ -50,33 +50,168 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>Sample wt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total vol: </t>
+  </si>
+  <si>
     <t>CondBlank1</t>
   </si>
   <si>
+    <t>GENERAL NOTE: ran on Shimadzu TOC-L at MCRL Rm 130</t>
+  </si>
+  <si>
     <t>CondBlank2</t>
   </si>
   <si>
     <t>CondBlank3</t>
   </si>
   <si>
+    <t>CondBlank4</t>
+  </si>
+  <si>
+    <t>CondBlank5</t>
+  </si>
+  <si>
+    <t>CondBlank6</t>
+  </si>
+  <si>
+    <t>0-50PPMC</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6, 7, 8, 9</t>
+  </si>
+  <si>
+    <t>Slope: 4.616, Int: 0.2526, r^2: 1.0000</t>
+  </si>
+  <si>
+    <t>0-3PPMN</t>
+  </si>
+  <si>
+    <t>10, 11, 12, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>Slope: 6.259, Int: -0.02583, r^2: 0.9993</t>
+  </si>
+  <si>
     <t>Blank1</t>
   </si>
   <si>
+    <t>NPOC: 0.08576, TN: 0.01556</t>
+  </si>
+  <si>
+    <t>CKSTD1_1PPM_CN</t>
+  </si>
+  <si>
+    <t>NPOC: 1.023, TN: 1.049</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_I5_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_E3_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_F4_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_C_PW_DOC_B4_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_I5_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_B4_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_C_PW_DOC_C6_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_C3_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_C3_15cm_20220613</t>
+  </si>
+  <si>
     <t>Blank2</t>
   </si>
   <si>
+    <t>NPOC: 0.1450, TN: 0.02779</t>
+  </si>
+  <si>
+    <t>CKSTD2_1PPM_CN</t>
+  </si>
+  <si>
+    <t>NPOC: 1.023, N: 1.015</t>
+  </si>
+  <si>
+    <t>TMP_C_PW_DOC_I5_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_D5_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_H6_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_D5_15cm_20220613</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_F6_15cm_20220615_DILUTED4mLsmpl3mLwater</t>
+  </si>
+  <si>
+    <t>Dilution correction needed</t>
+  </si>
+  <si>
+    <t>4mLs sample, 3mLs MQ</t>
+  </si>
+  <si>
+    <t>TMP_FW_PW_DOC_C6_15cm_20220615</t>
+  </si>
+  <si>
+    <t>TMP_C_PW_DOC_E3_15cm_20220615</t>
+  </si>
+  <si>
+    <t>TMP_SW_PW_DOC_H3_15cm_20220615</t>
+  </si>
+  <si>
     <t>Blank3</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 6, 7, 8, 9</t>
+    <t>NPOC: 0.1147, TN: 0.9744</t>
+  </si>
+  <si>
+    <t>CKSTD3_1PPM_CN</t>
+  </si>
+  <si>
+    <t>Checking method</t>
+  </si>
+  <si>
+    <t>CKSTD1_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD2_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD3_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD4_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD5_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD6_1ppm_C</t>
+  </si>
+  <si>
+    <t>CKSTD7_10ppm_C</t>
   </si>
   <si>
     <t>Sample</t>
   </si>
   <si>
-    <t>SW_Pool_T2</t>
-  </si>
-  <si>
     <t>Vial wt (g)</t>
   </si>
   <si>
@@ -89,164 +224,20 @@
     <t>DI added (mL)</t>
   </si>
   <si>
+    <t>Total vol (mL)</t>
+  </si>
+  <si>
     <t>Vial wt after addition (g)</t>
   </si>
   <si>
-    <t>FW_B4_T2</t>
-  </si>
-  <si>
-    <t>FW_F6_T3</t>
-  </si>
-  <si>
     <t>*two different glass thickness-&gt; explains differing vial wts</t>
-  </si>
-  <si>
-    <t>FW_I5_T3</t>
-  </si>
-  <si>
-    <t>FW_D5_T3</t>
-  </si>
-  <si>
-    <t>FW_SOURCE_HR2</t>
-  </si>
-  <si>
-    <t>SW_SOURCE_HR3</t>
-  </si>
-  <si>
-    <t>SW_H6_T2</t>
-  </si>
-  <si>
-    <t>FW_D5_T2</t>
-  </si>
-  <si>
-    <t>FW_POOL_T2</t>
-  </si>
-  <si>
-    <t>FW_E3_T1</t>
-  </si>
-  <si>
-    <t>SW_F6_T1</t>
-  </si>
-  <si>
-    <t>SW_SOURCE_HR5</t>
-  </si>
-  <si>
-    <t>Total vol (mL)</t>
-  </si>
-  <si>
-    <t>Sample wt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total vol: </t>
-  </si>
-  <si>
-    <t>10, 11, 12, 13, 14, 15, 16</t>
-  </si>
-  <si>
-    <t>CondBlank4</t>
-  </si>
-  <si>
-    <t>CondBlank5</t>
-  </si>
-  <si>
-    <t>CondBlank6</t>
-  </si>
-  <si>
-    <t>0-50PPMC</t>
-  </si>
-  <si>
-    <t>0-3PPMN</t>
-  </si>
-  <si>
-    <t>CKSTD1_1PPM_CN</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_I5_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_E3_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_F4_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_C_PW_DOC_B4_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_I5_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_B4_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_C_PW_DOC_C6_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_C3_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_C3_15cm_20220613</t>
-  </si>
-  <si>
-    <t>CKSTD2_1PPM_CN</t>
-  </si>
-  <si>
-    <t>TMP_C_PW_DOC_I5_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_D5_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_H6_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_D5_15cm_20220613</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_F6_15cm_20220615_DILUTED4mLsmpl3mLwater</t>
-  </si>
-  <si>
-    <t>TMP_FW_PW_DOC_C6_15cm_20220615</t>
-  </si>
-  <si>
-    <t>TMP_C_PW_DOC_E3_15cm_20220615</t>
-  </si>
-  <si>
-    <t>TMP_SW_PW_DOC_H3_15cm_20220615</t>
-  </si>
-  <si>
-    <t>CKSTD3_1PPM_CN</t>
-  </si>
-  <si>
-    <t>CKSTD1_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD2_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD3_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD4_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD5_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD6_1ppm_C</t>
-  </si>
-  <si>
-    <t>CKSTD7_10ppm_C</t>
-  </si>
-  <si>
-    <t>Dilution correction needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -610,19 +601,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AEBD17-6CC0-ED44-B8EB-00F06462890B}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="60.5" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,221 +627,245 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B27">
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -859,100 +874,127 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B33">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B34">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B35">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B36">
         <v>83</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B37">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B38">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>86</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -965,355 +1007,108 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+      <selection activeCell="A2" sqref="A2:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>8.7934000000000001</v>
-      </c>
-      <c r="C2">
-        <v>9.2637</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.4703</v>
-      </c>
-      <c r="E2">
-        <v>6.53</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2+E2</f>
-        <v>7.0003000000000002</v>
-      </c>
-      <c r="G2">
-        <v>15.7509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>8.6166</v>
-      </c>
-      <c r="C3">
-        <v>8.9382999999999999</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.32169999999999999</v>
-      </c>
-      <c r="E3">
-        <v>6.68</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F14" si="0">D3+E3</f>
-        <v>7.0016999999999996</v>
-      </c>
-      <c r="G3">
-        <v>15.600300000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>5.2081</v>
-      </c>
-      <c r="C4">
-        <v>5.3594999999999997</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.15140000000000001</v>
-      </c>
-      <c r="E4">
-        <v>6.85</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0013999999999994</v>
-      </c>
-      <c r="G4">
-        <v>12.1884</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>5.2286999999999999</v>
-      </c>
-      <c r="C5">
-        <v>8.6929999999999996</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3.4643000000000002</v>
-      </c>
-      <c r="E5">
-        <v>3.5350000000000001</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>6.9992999999999999</v>
-      </c>
-      <c r="G5">
-        <v>12.228999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>8.6166</v>
-      </c>
-      <c r="C6">
-        <v>11.522</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2.9054000000000002</v>
-      </c>
-      <c r="E6">
-        <v>4.0949999999999998</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0004</v>
-      </c>
-      <c r="G6">
-        <v>15.619300000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>5.2403000000000004</v>
-      </c>
-      <c r="C7">
-        <v>8.4842999999999993</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3.2812999999999999</v>
-      </c>
-      <c r="E7">
-        <v>3.72</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0013000000000005</v>
-      </c>
-      <c r="G7">
-        <v>12.198499999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>5.1173000000000002</v>
-      </c>
-      <c r="C8">
-        <v>8.7607999999999997</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3.6435</v>
-      </c>
-      <c r="E8">
-        <v>3.355</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>6.9984999999999999</v>
-      </c>
-      <c r="G8">
-        <v>12.106199999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>8.6455000000000002</v>
-      </c>
-      <c r="C9">
-        <v>8.9623000000000008</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.31680000000000003</v>
-      </c>
-      <c r="E9">
-        <v>6.6849999999999996</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0017999999999994</v>
-      </c>
-      <c r="G9">
-        <v>15.6387</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>5.1528999999999998</v>
-      </c>
-      <c r="C10">
-        <v>7.4782999999999999</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2.3254000000000001</v>
-      </c>
-      <c r="E10">
-        <v>4.6749999999999998</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0004</v>
-      </c>
-      <c r="G10">
-        <v>12.1625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11">
-        <v>8.6674000000000007</v>
-      </c>
-      <c r="C11">
-        <v>11.5433</v>
-      </c>
-      <c r="D11" s="3">
-        <v>2.8759000000000001</v>
-      </c>
-      <c r="E11">
-        <v>4.125</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0008999999999997</v>
-      </c>
-      <c r="G11">
-        <v>15.6427</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12">
-        <v>8.6786999999999992</v>
-      </c>
-      <c r="C12">
-        <v>10.9072</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2.2284999999999999</v>
-      </c>
-      <c r="E12">
-        <v>4.915</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>7.1434999999999995</v>
-      </c>
-      <c r="G12">
-        <v>15.7935</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>5.1361999999999997</v>
-      </c>
-      <c r="C13">
-        <v>7.2224000000000004</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2.0861999999999998</v>
-      </c>
-      <c r="E13">
-        <v>4.915</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>7.0011999999999999</v>
-      </c>
-      <c r="G13">
-        <v>12.0922</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>8.8002000000000002</v>
-      </c>
-      <c r="C14">
-        <v>11.788399999999999</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2.9882</v>
-      </c>
-      <c r="E14">
-        <v>4.01</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>6.9981999999999998</v>
-      </c>
-      <c r="G14">
-        <v>15.769500000000001</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1321,6 +1116,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007324DF9BA5F6B948938C142504C8F34F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4aadcd1f2a12dc9b07f6546b5e76248">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da8c28ad-5ac5-4047-b08a-f75bc24d91a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6457694f174ba676422feeebbff24cf4" ns2:_="">
     <xsd:import namespace="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
@@ -1490,37 +1294,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A701949D-1257-47EA-88EF-D14148793769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A701949D-1257-47EA-88EF-D14148793769}"/>
 </file>
</xml_diff>